<commit_message>
retrieved file 07 from github because computer crashed
</commit_message>
<xml_diff>
--- a/data/ICES_advice_history_updated.xlsx
+++ b/data/ICES_advice_history_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pstephan\Documents\github\ConservationStatus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B068A6A4-E85E-405A-AA29-24E1BDFD5CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCA4BA6-B855-4D7A-830C-6F240CC4FD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA0567B6-5845-49AA-A509-0E21DF92237D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA0567B6-5845-49AA-A509-0E21DF92237D}"/>
   </bookViews>
   <sheets>
     <sheet name="ICES_advice_history" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="174">
   <si>
     <t>Year</t>
   </si>
@@ -565,6 +565,9 @@
   </si>
   <si>
     <t>Catches should be decreased by no less than 36% compared to the average catches in 2018–2020</t>
+  </si>
+  <si>
+    <t>depleted</t>
   </si>
 </sst>
 </file>
@@ -1006,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B5EDF1-B251-4888-B89A-FA35557BC3F7}">
   <dimension ref="A1:J378"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I144" sqref="I144"/>
+    <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
+      <selection activeCell="F288" sqref="F288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,6 +1064,9 @@
       <c r="B2" t="s">
         <v>124</v>
       </c>
+      <c r="F2" t="s">
+        <v>173</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1084,7 +1090,9 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1108,7 +1116,9 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2786,7 +2796,9 @@
       <c r="C75" s="2"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
+      <c r="F75" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="G75" s="1" t="s">
         <v>43</v>
       </c>
@@ -2809,7 +2821,9 @@
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
+      <c r="F76" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="G76" s="1" t="s">
         <v>43</v>
       </c>
@@ -2833,7 +2847,9 @@
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
+      <c r="F77" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="G77" s="1" t="s">
         <v>43</v>
       </c>
@@ -2979,7 +2995,9 @@
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
+      <c r="F83" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="G83" s="1" t="s">
         <v>45</v>
       </c>
@@ -3005,7 +3023,9 @@
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
+      <c r="F84" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="G84" s="1" t="s">
         <v>45</v>
       </c>
@@ -3031,7 +3051,9 @@
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
+      <c r="F85" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="G85" s="1" t="s">
         <v>45</v>
       </c>
@@ -3681,7 +3703,9 @@
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
+      <c r="F110" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G110" s="1" t="s">
         <v>55</v>
       </c>
@@ -3707,7 +3731,9 @@
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
-      <c r="F111" s="1"/>
+      <c r="F111" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="G111" s="1" t="s">
         <v>55</v>
       </c>
@@ -3733,7 +3759,9 @@
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
+      <c r="F112" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="G112" s="1" t="s">
         <v>55</v>
       </c>
@@ -3863,7 +3891,9 @@
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
-      <c r="F117" s="1"/>
+      <c r="F117" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="G117" s="1" t="s">
         <v>57</v>
       </c>
@@ -3889,7 +3919,9 @@
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
+      <c r="F118" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="G118" s="1" t="s">
         <v>57</v>
       </c>
@@ -3915,7 +3947,9 @@
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
-      <c r="F119" s="1"/>
+      <c r="F119" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="G119" s="1" t="s">
         <v>57</v>
       </c>
@@ -4227,7 +4261,9 @@
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
-      <c r="F131" s="1"/>
+      <c r="F131" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="G131" s="1" t="s">
         <v>61</v>
       </c>
@@ -4253,7 +4289,9 @@
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
-      <c r="F132" s="1"/>
+      <c r="F132" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G132" s="1" t="s">
         <v>61</v>
       </c>
@@ -4279,7 +4317,9 @@
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
-      <c r="F133" s="1"/>
+      <c r="F133" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G133" s="1" t="s">
         <v>61</v>
       </c>
@@ -4409,7 +4449,9 @@
       </c>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
-      <c r="F138" s="1"/>
+      <c r="F138" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="G138" s="1" t="s">
         <v>62</v>
       </c>
@@ -4435,7 +4477,9 @@
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
-      <c r="F139" s="1"/>
+      <c r="F139" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G139" s="1" t="s">
         <v>62</v>
       </c>
@@ -4461,7 +4505,9 @@
       </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
-      <c r="F140" s="1"/>
+      <c r="F140" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="G140" s="1" t="s">
         <v>62</v>
       </c>
@@ -4773,7 +4819,9 @@
       </c>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
-      <c r="F152" s="1"/>
+      <c r="F152" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="G152" s="1" t="s">
         <v>67</v>
       </c>
@@ -4799,7 +4847,9 @@
       </c>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
-      <c r="F153" s="1"/>
+      <c r="F153" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G153" s="1" t="s">
         <v>67</v>
       </c>
@@ -4825,7 +4875,9 @@
       </c>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
-      <c r="F154" s="1"/>
+      <c r="F154" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G154" s="1" t="s">
         <v>67</v>
       </c>
@@ -5865,7 +5917,9 @@
       </c>
       <c r="D194" s="1"/>
       <c r="E194" s="1"/>
-      <c r="F194" s="1"/>
+      <c r="F194" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="G194" s="1" t="s">
         <v>75</v>
       </c>
@@ -5891,7 +5945,9 @@
       </c>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
-      <c r="F195" s="1"/>
+      <c r="F195" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G195" s="1" t="s">
         <v>75</v>
       </c>
@@ -5917,7 +5973,9 @@
       </c>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
-      <c r="F196" s="1"/>
+      <c r="F196" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="G196" s="1" t="s">
         <v>75</v>
       </c>
@@ -6593,7 +6651,9 @@
       </c>
       <c r="D222" s="1"/>
       <c r="E222" s="1"/>
-      <c r="F222" s="1"/>
+      <c r="F222" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="G222" s="1" t="s">
         <v>81</v>
       </c>
@@ -6619,7 +6679,9 @@
       </c>
       <c r="D223" s="1"/>
       <c r="E223" s="1"/>
-      <c r="F223" s="1"/>
+      <c r="F223" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="G223" s="1" t="s">
         <v>81</v>
       </c>
@@ -6645,7 +6707,9 @@
       </c>
       <c r="D224" s="1"/>
       <c r="E224" s="1"/>
-      <c r="F224" s="1"/>
+      <c r="F224" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="G224" s="1" t="s">
         <v>81</v>
       </c>

</xml_diff>